<commit_message>
Fix accidental re-use of CKR
</commit_message>
<xml_diff>
--- a/teaching/voc_data_science/topic1/lameness_Herd_A.xlsx
+++ b/teaching/voc_data_science/topic1/lameness_Herd_A.xlsx
@@ -366,17 +366,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>62376</t>
+          <t>76490</t>
         </is>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>79068</t>
+          <t>27588</t>
         </is>
       </c>
       <c r="B3">
@@ -386,17 +386,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>09421</t>
+          <t>04438</t>
         </is>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>76139</t>
+          <t>43840</t>
         </is>
       </c>
       <c r="B5">
@@ -406,7 +406,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>35357</t>
+          <t>84609</t>
         </is>
       </c>
       <c r="B6">
@@ -416,7 +416,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>93835</t>
+          <t>36363</t>
         </is>
       </c>
       <c r="B7">
@@ -426,7 +426,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>56215</t>
+          <t>25391</t>
         </is>
       </c>
       <c r="B8">
@@ -436,7 +436,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>79856</t>
+          <t>95016</t>
         </is>
       </c>
       <c r="B9">
@@ -446,17 +446,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>05601</t>
+          <t>91689</t>
         </is>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>96201</t>
+          <t>12561</t>
         </is>
       </c>
       <c r="B11">
@@ -466,7 +466,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>52996</t>
+          <t>93225</t>
         </is>
       </c>
       <c r="B12">
@@ -476,27 +476,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>83080</t>
+          <t>82422</t>
         </is>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>39461</t>
+          <t>49032</t>
         </is>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>83466</t>
+          <t>21352</t>
         </is>
       </c>
       <c r="B15">
@@ -506,7 +506,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>85934</t>
+          <t>22313</t>
         </is>
       </c>
       <c r="B16">
@@ -516,27 +516,27 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>57726</t>
+          <t>73246</t>
         </is>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>47112</t>
+          <t>91991</t>
         </is>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>59965</t>
+          <t>97764</t>
         </is>
       </c>
       <c r="B19">
@@ -546,7 +546,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>70204</t>
+          <t>50859</t>
         </is>
       </c>
       <c r="B20">
@@ -556,7 +556,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>00579</t>
+          <t>15092</t>
         </is>
       </c>
       <c r="B21">
@@ -566,7 +566,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>81471</t>
+          <t>93744</t>
         </is>
       </c>
       <c r="B22">
@@ -576,37 +576,37 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>30617</t>
+          <t>48412</t>
         </is>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>56724</t>
+          <t>70366</t>
         </is>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>15602</t>
+          <t>36418</t>
         </is>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>45634</t>
+          <t>03934</t>
         </is>
       </c>
       <c r="B26">
@@ -616,7 +616,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>73667</t>
+          <t>39143</t>
         </is>
       </c>
       <c r="B27">
@@ -626,17 +626,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>93424</t>
+          <t>79916</t>
         </is>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>19372</t>
+          <t>22707</t>
         </is>
       </c>
       <c r="B29">
@@ -646,17 +646,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>79697</t>
+          <t>72769</t>
         </is>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>79881</t>
+          <t>96038</t>
         </is>
       </c>
       <c r="B31">
@@ -666,7 +666,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>96883</t>
+          <t>23910</t>
         </is>
       </c>
       <c r="B32">
@@ -676,7 +676,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>61742</t>
+          <t>98581</t>
         </is>
       </c>
       <c r="B33">
@@ -686,7 +686,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>45874</t>
+          <t>51246</t>
         </is>
       </c>
       <c r="B34">
@@ -696,17 +696,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>09490</t>
+          <t>39597</t>
         </is>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>66669</t>
+          <t>20428</t>
         </is>
       </c>
       <c r="B36">
@@ -716,17 +716,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>97103</t>
+          <t>22117</t>
         </is>
       </c>
       <c r="B37">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>58343</t>
+          <t>57701</t>
         </is>
       </c>
       <c r="B38">
@@ -736,7 +736,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>49550</t>
+          <t>21573</t>
         </is>
       </c>
       <c r="B39">
@@ -746,7 +746,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>33203</t>
+          <t>65391</t>
         </is>
       </c>
       <c r="B40">
@@ -756,7 +756,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>19261</t>
+          <t>72985</t>
         </is>
       </c>
       <c r="B41">
@@ -766,7 +766,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>25421</t>
+          <t>90541</t>
         </is>
       </c>
       <c r="B42">
@@ -776,19 +776,17 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>92563</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>Walked in front of another cow</t>
-        </is>
+          <t>38417</t>
+        </is>
+      </c>
+      <c r="B43">
+        <v>0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>49963</t>
+          <t>25884</t>
         </is>
       </c>
       <c r="B44">
@@ -798,7 +796,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>33809</t>
+          <t>10974</t>
         </is>
       </c>
       <c r="B45">
@@ -808,17 +806,19 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>84645</t>
-        </is>
-      </c>
-      <c r="B46">
-        <v>1</v>
+          <t>14473</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Not being milked due to clinical mastitis</t>
+        </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>00089</t>
+          <t>79964</t>
         </is>
       </c>
       <c r="B47">
@@ -828,7 +828,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>91997</t>
+          <t>90530</t>
         </is>
       </c>
       <c r="B48">
@@ -838,27 +838,27 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>33500</t>
+          <t>26743</t>
         </is>
       </c>
       <c r="B49">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>48006</t>
+          <t>19258</t>
         </is>
       </c>
       <c r="B50">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>16550</t>
+          <t>57153</t>
         </is>
       </c>
       <c r="B51">

</xml_diff>